<commit_message>
Testing uploaded spreadsheet is valid
</commit_message>
<xml_diff>
--- a/upload/1_fred.xlsx
+++ b/upload/1_fred.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,957 +424,932 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>media</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>host species</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>strain</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>key</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>bacterial species</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>resistance marker</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
         <is>
           <t>freezer</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>phage id</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>plasmid name</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>box_number</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>storage method</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>project</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
         <is>
           <t>drawer</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>box_number</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>position</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>bacterial species</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>strain</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>media</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>plasmid name</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>resistance marker</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>phage id</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>host species</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>description</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>project</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>storage method</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>name</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>LsBTqfwTTbDYViDcGBFH</t>
+          <t>SmZUBXgNyFpNEQbaGnewTpvlBlX</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>WIiyrscccvKEVYSSOpgD</t>
+          <t>uGOPXXsf</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>PWLUhtGjSaQeOZzjrodd</t>
+          <t>lBqcuneLqbMhkJjWViMWZcoAEMJEHzOxGyGYqKSVNSOQZLTwXopzEmayJWveyKbYUUZwMejgPa</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>FKlsNVkLVfHrovcjZzZs</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>aizYpPgJSCXtWNAJUsRp</t>
-        </is>
+          <t>2005-08-28</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>7508</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>DaJXyPJcEWBRxipLxDOR</t>
+          <t>qjscda</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>NCULCGDJxsDlCsoKaOVS</t>
+          <t>ZxZTOTBibkBYYrPYMSRtggVvIsNAtNFUwJaRWdulWSUFOzarWvuPC</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>lGtoMavyAYxrJKQCjPZv</t>
+          <t>cSKk</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>kJtRBOkmeOisMQFGpQts</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>GUzOkgtLTdJrQzKaxsHA</t>
-        </is>
+          <t>DbFMpbOecTTTfaKcNWPfRgdpFmlzOoSxPMrOdbZkxdwrhItosdHKtgbXiYMijYOhbAwYcFhnoYiguWlQQFGVyoezyoEseeE</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>7058</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>cEyaQFcUZTmchaBgduKa</t>
+          <t>ZppE</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>wDOvjNaRHtRORuAiiUUb</t>
+          <t>XYSfFQBLmaEgyZUPGeccLDbeUrcwsZrUZhzVgKl</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>QnZmBrzeXtShzktSBFLr</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>XkvFxtJdAwWUCmToOvFW</t>
-        </is>
+          <t>udTPlFCRxNHDiOrqtW</t>
+        </is>
+      </c>
+      <c r="N2" t="n">
+        <v>1383</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>EjJFibPFzfbtPtkgUvnA</t>
+          <t>OaQmVLwVmQWSpglQqBRZSVvWfFngXEVGdKcpyCVWFjIOkVkwWdaoAZOxYnKYJqYkRCORTsXDLrpNudJvEbJyglQZSHmvFHPiCdDTCwmNskmwNqFMrLXUZcCljcsMTuIzuZCrSexsIivlWpDEhGDq</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>iTfPNKCyuuCgyAdaecuE</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>hIKaXrLJTrQnPqsCPOjJ</t>
+          <t>NgjrwornfgXdOiNUNTyLiPABRpTqULdvZMwFbfFFBpeCjoVEpHIbWjidVUlNPkNzIKBdBaGcRIhonGBiDjkZSJu</t>
+        </is>
+      </c>
+      <c r="Q2" t="n">
+        <v>588</v>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>i</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>QletMPpAIuilVyapvUMz</t>
+          <t>ESEtpAbZuPXQZvEaJkNyKOUqKXdOXbgJHIrMrHwOfoxyNc</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>aUTCdvkGmiPLmttjmUGg</t>
+          <t>nhbDwMLyZjVfhHFCNpXiHBYcymddeDaKEJJqMTTeDo</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ACpFTVcXEfIxfIAwKopR</t>
+          <t>W</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>UTrAHeaTewYEablRDfCL</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>kWalPEwdZxlGvJfTRydW</t>
-        </is>
+          <t>2000-12-14</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>8620</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>EiuvrxOYCNEvlfLpkwAq</t>
+          <t>wwmnUvZx</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>gMZpryTIaERcamLLoGap</t>
+          <t>vGHBKHAyCUNLvXJutESEFrCGjBnyTDOGbItJQcSHCBJxAGfgVqjUw</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>rWiambqPAmwUZFuDGIpa</t>
+          <t>b</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>crghNxdjUBtqEgKbnUYj</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>HXreghQerrspNmBeyIAC</t>
-        </is>
+          <t>HPXcOFoDElamjzHXKDQgKvU</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>9270</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>iBPaqlbRSwRSIpHtMzKp</t>
+          <t>nbiIqPlkf</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>wSQdMkVckkSJzHcCnJMJ</t>
+          <t>wWVfFLqWhbAwtOaZreiPrxsUe</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>ezbJRyIyevPhPoJyfhpu</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>IYcYhqCRSlKpPfEhPVFE</t>
-        </is>
+          <t>mdbwCoKnSGIpbQyIlNEAHxWldCKANWLtySHQZNvLChpYrVbQniwMOvBpAojhLjTiF</t>
+        </is>
+      </c>
+      <c r="N3" t="n">
+        <v>4243</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>bntcvYhPyHgrcHYNyPGB</t>
+          <t>RAGyFgHFDNRTbzGJnmLEyMKRLuQMznLbYwTZmJOJjRvuGRYlnqvODuLNwMEdMEBIAPiooSBpflXEYBGMGNyILKpzdgzoVaZIPPdxQMoeGblDrxBEMVqR</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>hCsXeWivDzZYsDmiQrtj</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>nyakWyQTMKAQAuAwUHUH</t>
+          <t>UdEJKThQazPxICpSrqoWStjHfbYJFHRKTzIVvXxgTteBKjBgIHtanTrzQggsdNHdndzdsHEYUkZJ</t>
+        </is>
+      </c>
+      <c r="Q3" t="n">
+        <v>6607</v>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>rXyzVXgNeJ</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>vKHrMlMTthIXLXrcEaEX</t>
+          <t>EutFtcxelvvMcvrmAGLWJHnGNhIMImNPuddCZxLmJWKQIRGoIQmPzWGRvbeBDIHhQhajIsUb</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>shIBXEFzKeJVgaHMkCvM</t>
+          <t>rbMhVUyFqvVVlxzJRlvXNrDdxRZleutNpmNaUzWRimIjNPMOPDmUlWihLTmcoSEcyAhbLCcGWXjJsomfmrqPoHQiAHyWHhm</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>XdQWQzLuUDDLxTMBpqMh</t>
+          <t>NvhvcQrLTzpsdUeTveQAQirNFJRtoElqdDAG</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>TRjpjmNzFOxXJRNPvBSo</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>cbHuaBZVyFgkpUJWyRdi</t>
-        </is>
+          <t>1981-10-18</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>3445</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>QtDzmJHeruAtqwWQRYLR</t>
+          <t>uD</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>UCmDVzrhsmfBZhEASvfz</t>
+          <t>XbqiVxMCuHskBVJMMFkqNOxEamSjnoiVkTWfynXDtqJMY</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>RoTtDShsPFqoiTYQHTbH</t>
+          <t>ocsLUTQAJsQ</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>DIHUHkDRGYrUXGLpymIS</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>yzkhCigaPozzdLnjRCNi</t>
-        </is>
+          <t>MEpdGTKJRsrrBSEHgLLrdrRIWsjeuTjqAYRwIBUOqnBliHsDBDSFknUreeUHdwwrEABgZHmhdAwqELcDWsNwqkiA</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>9241</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>FeqdRHYjerjKiWBpBOiz</t>
+          <t>MKzZwcPXXz</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>ntPDjiJlCaubljSyXTIn</t>
+          <t>ngfvmyPdCqicivmQHJAyPgopUaStKHBtIBTdnwoLtcRzamTqqdOTpcUoGnvcpdAYkyvmIuPXPUjXnraDlXO</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>fowOZIXAbrOfWAyrUMjg</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>pghoOgHkmOxXoBhDHHjq</t>
-        </is>
+          <t>EqJHSvmRvqXKAvgOTYXgpADVKvdGEEiuDUtbSgemaoDfexitkcsJlVLTGoSwdxOBOukgVDyjKLMNjznFBQaUzjrDlQTv</t>
+        </is>
+      </c>
+      <c r="N4" t="n">
+        <v>7342</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>ieVsuAOyFhvVUiVzgWUH</t>
+          <t>TcCvviZKqgjDLnkYBdEEQuGEcCwjxBteILbopjiawDqCeqUdXoxPoDzLjVlhjPRFdZkgyoqjHtSXhwsXieAQMamdSkfCjXuiFIDZzoxQThYbNBSdJmtUKFRgpmOyTtyLAP</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>CNwivZEJxYwuEpwbNeJd</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>bcvyYKnqyZlrEslymsGc</t>
+          <t>GKIZlVoMUrLZ</t>
+        </is>
+      </c>
+      <c r="Q4" t="n">
+        <v>9157</v>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Bv</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>YiXAjoSyRGshYYvYDzcz</t>
+          <t>WQRFBvEUQvWRElKRPiwkiejcoRBMbkfTaRJpviNhsupXVteyizvSrnLgelQEn</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>lSGBrvLkLzIkpaKHjAPK</t>
+          <t>rzrOJizlJNIkzXLgNQBxaxKpI</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>kEDdDlFUGFmXipuPfnFA</t>
+          <t>LSjycBfWxknRJOGNORLkDpjwKADyGnbVSCBMDSaVEtRUegoRAgSwpZTZJsgBJkGhohoSrI</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>qvAKIoBWYxcIblToxclp</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>ihuXNxEuIAsdFcBwJTxc</t>
-        </is>
+          <t>1978-06-13</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>9059</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>oKrNjdnZoTNQPqjAyuVi</t>
+          <t>IFZwfyeu</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>hhCiVMqoaSoXLZPtwOIJ</t>
+          <t>gwSkZDTFIPmwSZycBziuSMemTtVvWjxAPnOcysiNVRNqB</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>qzLQgKHKyVdLjKoodOSB</t>
+          <t>ZJLKDwLwlIlwQnqTHIO</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>RUABgrHlDTZyJVPBcizX</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>cxXMIZaWOMxVfuLmJNxV</t>
-        </is>
+          <t>fCYLajDRldrcywdhWhQrAWfYjsfRIsgDVTEHqZdcGUxsfbeUdfnu</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>5096</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>IlgWTOLRqtenhcFqIfQp</t>
+          <t>xvHzKTR</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>qIRUBZaaufBYyEiIyGSu</t>
+          <t>QXLHt</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>YsEuxAHuhePHYiqlwnbj</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>qIrwLgIwZIcoqaTWhByB</t>
-        </is>
+          <t>rgBWXCJkGyAXYdAQgKeMQAaatZtJtRoxRTcgxfZIssPfggkDuWporcghaAjSTNNnyaoTzqBeztxHImQZJRwDKQJPqJEpzMxAc</t>
+        </is>
+      </c>
+      <c r="N5" t="n">
+        <v>379</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>ELqsQYzKBRzbzCWNgFFo</t>
+          <t>WHegUSNrhwcJLhShZgzlKJPLJDBIEixjPNpTAWfjKgQJbWOsrUJVRdxGxvlBjUfUHQCLMIbeEEFSfnOPlwLQSvFXLITpJvanBwThQmTlcVSNCrwjMOYRqGMcKebqUolpt</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>PPlysDxSFfpqEOfacPqn</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>bPmtfGAsAlywRJZJOrBn</t>
+          <t>QIaQ</t>
+        </is>
+      </c>
+      <c r="Q5" t="n">
+        <v>5607</v>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>ut</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>yGsiNprqRwncwtIzMuPG</t>
+          <t>jGVHURzQQrJpTSlikdGytYBCnhuyFfczeUMPWGkrFBWWAFYkUi</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>pktfnEBOnFvtTrQorviN</t>
+          <t>NYfUZQHVOlsNHkdQxrgDBQQy</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>jalMtKIkYKCBhFJPxbgU</t>
+          <t>EVoHuSzbnWpIyVLxozV</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>RpbyqKBhHZhiNuiFuvZl</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>tCbJFxYnsQsSLubTDnnU</t>
-        </is>
+          <t>1976-08-24</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>4831</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>RaqHNnMYMgzogCvXXAim</t>
+          <t>NHlxf</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>qcljRaGdHicfGBFCNbdI</t>
+          <t>JIcpAhJGkxsZearCNXmDITmQhZmuVlPVFTWKgNxnQLzfaEunXEZshyzLDKMFlZhnoGFjZdABzheabkqxHywuSRCFMJdOmEUybGwx</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>siWHgfLDRsYtnAReyuao</t>
+          <t>SpVgZsMpgZKQCzbzC</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>rpmxBAjFWgIdIgFoDvyP</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>VbyHFDnoQwLzXTLStgMn</t>
-        </is>
+          <t>swXIVbotXJUHIsoDGdhidQgphvNKwyqEyVCnFTuCjrYunfINRyGL</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>8873</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>SpyIzZDWjvJTXrApceYG</t>
+          <t>u</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>girFSfweauDEbRjkJgOd</t>
+          <t>HEpQcJrFQFXADNyVWznBGphurrdqEGOpbAPbmlogXQIWqntBCueIRBvYVBRPJEyPrJqjhAwPjJOtScjcoOVRuyQejgTTVhM</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>cQdaeCJosemgLgHAKPcK</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>DFRqBfrzoFsYUVKkqeZU</t>
-        </is>
+          <t>ibIMYiOrlrDrYfiSxoPPHCsZmq</t>
+        </is>
+      </c>
+      <c r="N6" t="n">
+        <v>5564</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>lIJuXhgpBLOMcuXlSRgI</t>
+          <t>CGnEZUgZWqqzTppjVWxJIIrLgUPbnoyDlhNbpUkLhTlsFebwPhevDgpfqBmhIPLVRuvHGtzuFNUXoHxLgghhEIxJiQeTQQJMsLRESJJfbuozYHwevynVwKKxORZPDjsSxXFCCEFiJNCARIsO</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>vIRaySYeitCgMpsnVVkH</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>nIfyZoaSZqmQimdyljMJ</t>
+          <t>FVjRpthXhnfqbLYcKIVFBBAlQQTe</t>
+        </is>
+      </c>
+      <c r="Q6" t="n">
+        <v>8587</v>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>WYlljy</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>pYcgmzIezZfGVHAVRsMQ</t>
+          <t>RVrjUWc</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>evmvkOCjEKjMMMQSgOcu</t>
+          <t>aMBzHOSUXPk</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>fSXwLRdpZexGbdgQGNBa</t>
+          <t>lbdKLuGRInHWeVlhxPJSlmlhYgC</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>sOZjhVLViYqrVkcPmHjP</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>JkWCXDlXtitPxolsvraW</t>
-        </is>
+          <t>2020-06-11</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>616</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>jkIyCYLAAEbfLGiiVCFw</t>
+          <t>YJsTqAKuLG</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>GKWAnEMQqNYAppTuAHpR</t>
+          <t>bScHVRbziaHrSHCLuHngvV</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>UeOtwJvNJDatiEDccZxE</t>
+          <t>Jksz</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>frjTYoPKxvfBvGtgEnHv</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>ANjVDqggCFJFLxAaleMg</t>
-        </is>
+          <t>lydbMnDWFVcwEabqQBADyyJZCSFbDgRCDtNSrfRIHCrFxvNfjlrlfUJmBFnbfjzokIqSNZYSCiyZuZAb</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>7960</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>OHqJjItyggyphcMPTvlm</t>
+          <t>lXRUcYY</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>qzkgfyENtztsiWirpOSO</t>
+          <t>njTVmcJLYSMG</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>eUNbKOMKZINMPqyunBke</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>PeEjygapoaQCUZJTbjvj</t>
-        </is>
+          <t>HUFLTkQdgrjW</t>
+        </is>
+      </c>
+      <c r="N7" t="n">
+        <v>6016</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>IJFVUbVetbSSlFQqAJJC</t>
+          <t>CyPOrulljGiXdnygJoDuyuIeZxlCkoVqntSGuziRgbQzVEYIERVJXqNZUIGogPlVuMhINzeONcvKZtpQdrXkXAIgIlKWsnwrxJXdezpHvtzzqQGDzPCyopif</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>llEzVNtlfEhuOHDWXrJq</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>yBkBwuhoRkUfQLeUuxwe</t>
+          <t>DWGkOuAUAuNtnPZZRPbUhPkjYnXlDWSJUTZomgcwQn</t>
+        </is>
+      </c>
+      <c r="Q7" t="n">
+        <v>7836</v>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>cXMiNqvMkB</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DvrCcxiHXnZBqNWWGaxz</t>
+          <t>rlVsSjbtWgYrzPSILkLbnGXqfeKVzhGBuVlOQKtajKvhLvFxvhVOJIOREeLdbTzRvrSlFX</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>CMtfIgMTODXfGBIBmJqB</t>
+          <t>ivxISxSjblbtvGZMhDIwPcAXcragtPSVaGfglcIPbElTWXqkgqKbKMGADIBUCQaGEkRtCDvSkINOP</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>VHaQTdtojyvSPDoQkkIL</t>
+          <t>CkBGPUXSJPBskTkGZSbxpOibAjaBWCivoNFQIon</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>eVHALVXqoFDCDSJucoaS</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>MnAtsSsWWYavXeQfWzwI</t>
-        </is>
+          <t>2001-01-24</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>9877</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>GeGCboLSRlntwfHSiSsU</t>
+          <t>ywCu</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>AzHQNGyrxtLPKufLHJqy</t>
+          <t>rTwMeXVDdwySSExUtPzLhslLsjflVKJvlgKHnOFnWLqTZevTBNOVxkjVREbrUyMaVhgHWKTwEKrSDJNVtivNzGqnq</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>xfrkXncttNDIrqAgrFFF</t>
+          <t>D</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>KJlhNulmknfzPSKrvxND</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>CWmncajjXrpXJaBiZmyN</t>
-        </is>
+          <t>pcvnzgMpqVnrPmOhXjIuZnmxHROEUSkPeSksXNjYYiJTDv</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>878</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>MJVbzpTvsayojyACcITt</t>
+          <t>F</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>qbySQhKtdHCVfhCdzAOe</t>
+          <t>tQplIdNTFNfMphhkkWKNaEKNNRBjoBWHdhzkWAhxsoCNWmchxBaSDzTwEHpSjttPaAWZhYimVZzrmRNi</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>OYUKSeGyzBlwGvGkPfSv</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>GeNBKNiwhlpywKtnMTMJ</t>
-        </is>
+          <t>QbQzZJSJQPENELrdeXuBrHDAiLeGGauSHxzlVeQnMhUYLftyvFKEcyiaieJFwvRTWxAnVMMWXSnvTxIHAoxJzUyGrU</t>
+        </is>
+      </c>
+      <c r="N8" t="n">
+        <v>5741</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>IkkCvbqpKVYChYhNMVWI</t>
+          <t>tqVJYeZDCjlgDrOyhHbRPmUVYQkvWkagezkymwBBzvpKzqNKxseVtpyKfjQEZdaAxGNiPCaWIahgyakoWYxRkLKadvSRviVvfanZFnugfmwwmEZbvyOlrdNiBJqqhzap</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>XuErNlHczRSRNzTXslJk</t>
-        </is>
-      </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>gAcLCbaPlYkscwBqBByB</t>
+          <t>phNohLdEyqRhfUYvcVAZfBwMHrlTG</t>
+        </is>
+      </c>
+      <c r="Q8" t="n">
+        <v>5552</v>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>fpSC</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>aVsKlEhvwZrfYWXtfkXA</t>
+          <t>qfNCSJuySdkOOLSVgeWjvGkYmjDHMAoaLpTVKLOvXaYQFrsKuatDytRLVggYYzUVpOAorZVbCIoPDqMWvfOZEMYVyq</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>dTdiHKRcwzBwOYBGMbbC</t>
+          <t>IinrUGdVlJ</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CXFYImUDPnUYcvMpUZzI</t>
+          <t>SYjdDNzJdUjlZvIQGQTDzEdfMDMGpgbvEDRaMHBIeQzoDkimergmSICGbEXYBrQJVqWVzaYWHkMiwotMqUuuwSDnBtFmSc</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>SaJGZVDuMtagKWmMEnCT</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>ZWwymbACbJnPgydPATBQ</t>
-        </is>
+          <t>1972-01-11</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>4121</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>JamzYDLUrTMjznasCWDb</t>
+          <t>HAI</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>ejvyQztDSnAYdOWmHVhc</t>
+          <t>FmbiuZAHwxC</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>FKXEYyKBspYjtkSNVydJ</t>
+          <t>Jcgkqnk</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>CRuOSkFvCVkIKLCRwuPL</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>NtFgRZDKyIwpWZijNPNr</t>
-        </is>
+          <t>cjqLoaHUFCKtWThumXuzDfbplsmaiLKeuQcvYfVSPsjtKHFMhaBuXsvedvAZexRzeTXPar</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>4639</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>fUQezgXUpnvcALXiLvAd</t>
+          <t>UjnYEL</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>hVbrjpNqeYDLSSadFcFQ</t>
+          <t>YcUARqv</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>OgTAxMAvlBdhnNtjxzVi</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>SCEsnprqqeOinjpKDhDW</t>
-        </is>
+          <t>whpokbJJtvPlQIAyfcaNsyjNnHchnGkmwTYebHntIOdjDpwzEyxHzTOBasXayegXbTIfJKAaRjFur</t>
+        </is>
+      </c>
+      <c r="N9" t="n">
+        <v>6086</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>QfUmIKfghXhHOIAgGrQn</t>
+          <t>rUkNiuGWxWUMZyVNEadNnRuJlVoHSsafJeqHYeinIRuUGEwTNyeNdGAnwxEEJYyxaJqnVXLbHIJDiRFpXsiZwVpZDkwJgbRpetiMxxZhwHfuzmTQpekDQsHIRXsdbLEngEGLgSSvPgTiZNNmHfwOPkUhBZkniONgKVRrbkTKIINpSRDJIXSGKqEfudiTrzzPX</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>iOwVtHdmbjfFkjgDDKfQ</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>BvFUQsirvdlRXdtRHGcn</t>
+          <t>wXRYPgGpSYSlLOiSaPfqFuspwzRciibXJzqHHikRcMhRgtSNzgIeWAZepjkAgDxfNyBIiDyemOIINUkVobMFhkYWKD</t>
+        </is>
+      </c>
+      <c r="Q9" t="n">
+        <v>1257</v>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>sxpq</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>cFcWyrBgSIcCNjVmegAZ</t>
+          <t>gTJvUTWTGvVcnpClQBFntKGNzNpltnqcTROkCvZksDkNLfiqzCgTkL</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>eErGwZVNTiHuOcSIhulq</t>
+          <t>HbzgSXsEDBzyTYTcVDZvGOkAsUmPvroPBeRPndhwsaVkbJABFhnQtiRZiUumRShKJREFjWzEnZAvDLGrdIrCLi</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>fGxGmlBgJTAWGTEEWAJP</t>
+          <t>FiyvNwopXIRiWlvPaEsGVhqNVdesOGxYmpDCEUUcNLpATQpLpiT</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>CYfuUtIMFmiogRPQLUPJ</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>xPZvZGMKUeBrVfvKTBDO</t>
-        </is>
+          <t>1992-06-14</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>5081</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>bDNfaCacnmLtdnqcPIZb</t>
+          <t>x</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>cZpZwoGtsUJEOXvEEDUj</t>
+          <t>jzRfULmzVzONHSxaFRXGIgmVsaKjMgoXksDGtyAelFLsSnnQyZIGNlH</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>qTGxafFlHOoRazbvHRPj</t>
+          <t>eR</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>UtVZrLktKzoKqQmaVsZx</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>psXhBWqbmtjQqHJsmBUl</t>
-        </is>
+          <t>LPherVGVGUSaPzevsAjUbaqpyqzjNNhBBDyWDrtvuCwYvGscdUisJcEJbPfpiIvylDmXatGThtIsvpWplsMNqU</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>4164</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>WHFaqudzRcWJoKifjzmf</t>
+          <t>YzNn</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>ZVqjpcDWUbPGYWquGfux</t>
+          <t>BnxtjVucvQwHKZOoaVBTxfDwagOYTkYiflhXxdnzIMKJWeBMftyrWeoCRzlAybKUtuRtpoGdEFyneHfPNHvHlNXZ</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>LZdKeCrjCoUNRERYhdFN</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>EKhXILLRgRHrxkYVvvlw</t>
-        </is>
+          <t>IkIxmJFTOINEfCWXLLlOSPJJKNKQMNVczxeeRuvHutgkBVomgsORPvfWSXFPSvKC</t>
+        </is>
+      </c>
+      <c r="N10" t="n">
+        <v>861</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>mOvjTpmCAMCJxBSHJAjR</t>
+          <t>yaaEkbuBsqVPVFwqfNCKfYNLZQtDpcPJWjfQxnVBbRboUMQmBvrzQObwkyXkMMcNSEEfcnFwvtHmZFZllFUBDJrcmMeSKChhYoMQffdPYgSloirySCY</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>LEMwLQrNNoFfwtlDRiaH</t>
-        </is>
-      </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>zqVwYstJzkimSrHjqBFS</t>
+          <t>NquspPtCRgqgaDiPDkCDyBQPUusYyvYna</t>
+        </is>
+      </c>
+      <c r="Q10" t="n">
+        <v>6229</v>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>p</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>MvacymdUhQFbIlTkZVHz</t>
+          <t>jTUXkfcANKBBEEdjLImQaJenkNxVkVloKytxUjpsfiOFeMZxqnHiUZsWKaNbkuWFrQuOgHdUh</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>sXnUbexpWhvoDhbMgUhq</t>
+          <t>NTkNwyoWphkcuVQcNfjYmPHjjhVUxmjehacJdXZBRpLwOzcPZfwTaKzRUcgqFbkpTKbBL</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>dqBpZSxHIDZSvqDeHdJi</t>
+          <t>wJBkRMgaiUgTTKMhtuSALdkERcSSXWkyGnGILzysEblkbzamqOUXdWznYYi</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>dvsuBETGpkXdhhbButGw</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>yjszBNYJbJDPGiMKOuhm</t>
-        </is>
+          <t>1983-02-14</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>9107</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>gDjDGPudFJQeqooksZRv</t>
+          <t>h</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>scQsfizrahdHSlpeMMOh</t>
+          <t>QVtWmhlr</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>tyKZHmLIhKXEbsbnXsla</t>
+          <t>RVCqzUFXGMibsqBT</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>EkDCOojosXzjlbvipMUR</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>PKqkqwifLAWtEppNkUoO</t>
-        </is>
+          <t>cF</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>3611</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>rtguqdGKSqSxMzkWIzDt</t>
+          <t>IdA</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>odAWYtJCCWLKdAfySIZu</t>
+          <t>mfFWHrzqpyLuRulaKIZEOXPZyIofyqvZNdmNLLKztPZxSxnRQpzmbTJAdtnMBDsRNPyMRs</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>HMShVpNjrnMmnchUgQdm</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>dgcLIiWQqTTavceeyLJs</t>
-        </is>
+          <t>iemynmRBLMFhlErWCaDrARBeApMqCVHGXMVprULWyevzxmVpIwUFQqXuwdpBDnjOithMezQECnDM</t>
+        </is>
+      </c>
+      <c r="N11" t="n">
+        <v>1066</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>NfvlKRKHAAqVvvUIqmbs</t>
+          <t>NUNtTIcAteXXEuWPxxRJvNbJkoVvnAhoFGnxuraPiDolvyuOleeBnEPHbDPCFhFjbktThAyQqWHdDONwxaeHLDquOpycYTtzELdJoKxgQrbOIvzLoDJNqAA</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>bYLtPnBhcsCLQVhRjypc</t>
-        </is>
-      </c>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>PualQETgmcsqUrSSFjyq</t>
+          <t>PPZilBIDWasTofXqKrxLwUdxQoWJrcqBOIxhQiNZCDmFsBKxWeXVIwIReMcwxKSurbCRtOnZ</t>
+        </is>
+      </c>
+      <c r="Q11" t="n">
+        <v>502</v>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>blsQiP</t>
         </is>
       </c>
     </row>

</xml_diff>